<commit_message>
updated graphics and sprint burndown chart
</commit_message>
<xml_diff>
--- a/basic backlog.xlsx
+++ b/basic backlog.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/karlypeckham/Dropbox/Grade 16/Semester 2/Senior Project/Senior-Project-Networking-Game/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{29427983-1F0A-584B-A6E2-358AFF5BAD2E}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{399E0C6E-2BD0-6049-9EFB-C7737D5C7DB2}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5400" yWindow="460" windowWidth="22940" windowHeight="17460" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7240" yWindow="460" windowWidth="22940" windowHeight="17460" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1425,6 +1425,35 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Sprint</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> 3 Burndown</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1463,9 +1492,6 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
-          <c:tx>
-            <c:v>Sprint 3 Burndown</c:v>
-          </c:tx>
           <c:spPr>
             <a:ln w="28575" cap="rnd">
               <a:solidFill>
@@ -1480,30 +1506,36 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet2!$G$79:$H$79</c:f>
+              <c:f>Sheet2!$G$79:$I$79</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="2"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>1</c:v>
                 </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet2!$G$91:$H$91</c:f>
+              <c:f>Sheet2!$G$91:$I$91</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="2"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>63</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>59</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>41</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5005,8 +5037,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A6:J91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E60" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="J75" sqref="J75"/>
+    <sheetView tabSelected="1" topLeftCell="E65" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="M96" sqref="M96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5450,8 +5482,11 @@
       <c r="H80">
         <v>3</v>
       </c>
-    </row>
-    <row r="81" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="I80">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="6:9" x14ac:dyDescent="0.2">
       <c r="F81" t="s">
         <v>109</v>
       </c>
@@ -5461,8 +5496,11 @@
       <c r="H81">
         <v>5</v>
       </c>
-    </row>
-    <row r="82" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="I81">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="82" spans="6:9" x14ac:dyDescent="0.2">
       <c r="F82" t="s">
         <v>112</v>
       </c>
@@ -5472,8 +5510,11 @@
       <c r="H82">
         <v>10</v>
       </c>
-    </row>
-    <row r="83" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="I82">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="83" spans="6:9" x14ac:dyDescent="0.2">
       <c r="F83" t="s">
         <v>113</v>
       </c>
@@ -5483,8 +5524,11 @@
       <c r="H83">
         <v>1</v>
       </c>
-    </row>
-    <row r="84" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="I83">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="6:9" x14ac:dyDescent="0.2">
       <c r="F84" t="s">
         <v>111</v>
       </c>
@@ -5494,8 +5538,11 @@
       <c r="H84">
         <v>5</v>
       </c>
-    </row>
-    <row r="85" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="I84">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="85" spans="6:9" x14ac:dyDescent="0.2">
       <c r="F85" t="s">
         <v>114</v>
       </c>
@@ -5505,8 +5552,11 @@
       <c r="H85">
         <v>1</v>
       </c>
-    </row>
-    <row r="86" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="I85">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="86" spans="6:9" x14ac:dyDescent="0.2">
       <c r="F86" t="s">
         <v>115</v>
       </c>
@@ -5516,8 +5566,11 @@
       <c r="H86">
         <v>1</v>
       </c>
-    </row>
-    <row r="87" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="I86">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="87" spans="6:9" x14ac:dyDescent="0.2">
       <c r="F87" t="s">
         <v>116</v>
       </c>
@@ -5527,8 +5580,11 @@
       <c r="H87">
         <v>20</v>
       </c>
-    </row>
-    <row r="88" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="I87">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="88" spans="6:9" x14ac:dyDescent="0.2">
       <c r="F88" t="s">
         <v>117</v>
       </c>
@@ -5538,8 +5594,11 @@
       <c r="H88">
         <v>8</v>
       </c>
-    </row>
-    <row r="89" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="I88">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="89" spans="6:9" x14ac:dyDescent="0.2">
       <c r="F89" t="s">
         <v>118</v>
       </c>
@@ -5549,8 +5608,11 @@
       <c r="H89">
         <v>2</v>
       </c>
-    </row>
-    <row r="90" spans="6:8" ht="32" x14ac:dyDescent="0.2">
+      <c r="I89">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="90" spans="6:9" ht="32" x14ac:dyDescent="0.2">
       <c r="F90" s="1" t="s">
         <v>119</v>
       </c>
@@ -5560,8 +5622,11 @@
       <c r="H90">
         <v>3</v>
       </c>
-    </row>
-    <row r="91" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="I90">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="91" spans="6:9" x14ac:dyDescent="0.2">
       <c r="G91">
         <f>SUM(G80:G90)</f>
         <v>63</v>
@@ -5569,6 +5634,10 @@
       <c r="H91">
         <f>SUM(H80:H90)</f>
         <v>59</v>
+      </c>
+      <c r="I91">
+        <f>SUM(I80:I90)</f>
+        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
committing this so I can switch to a new branch
</commit_message>
<xml_diff>
--- a/basic backlog.xlsx
+++ b/basic backlog.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/karlypeckham/Dropbox/Grade 16/Semester 2/Senior Project/Senior-Project-Networking-Game/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{399E0C6E-2BD0-6049-9EFB-C7737D5C7DB2}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{FEB963AD-9A97-6745-AEA1-BEB22263556F}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7240" yWindow="460" windowWidth="22940" windowHeight="17460" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5860" yWindow="460" windowWidth="22940" windowHeight="17460" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="145">
   <si>
     <t>Time Estimates</t>
   </si>
@@ -389,6 +389,81 @@
   </si>
   <si>
     <t>Changing resolution and doing Android/mobile switch</t>
+  </si>
+  <si>
+    <t>Karly</t>
+  </si>
+  <si>
+    <t>Nef</t>
+  </si>
+  <si>
+    <t>add edge bubbles</t>
+  </si>
+  <si>
+    <t>renumber edges</t>
+  </si>
+  <si>
+    <t>tie edges to backend</t>
+  </si>
+  <si>
+    <t>scrolling boxes</t>
+  </si>
+  <si>
+    <t>click and drag boxes</t>
+  </si>
+  <si>
+    <t>trash can image changing</t>
+  </si>
+  <si>
+    <t>score box updating</t>
+  </si>
+  <si>
+    <t>checksum front end move numbers</t>
+  </si>
+  <si>
+    <t>Change resolution, switch to android</t>
+  </si>
+  <si>
+    <t>Dijkstra testing</t>
+  </si>
+  <si>
+    <t>Checksum testing</t>
+  </si>
+  <si>
+    <t>Segmentation Backend</t>
+  </si>
+  <si>
+    <t>checksum explanation</t>
+  </si>
+  <si>
+    <t>binary addition instruction</t>
+  </si>
+  <si>
+    <t>pop-up encouragement</t>
+  </si>
+  <si>
+    <t>Dijkstra explanation</t>
+  </si>
+  <si>
+    <t>pathfind instruction</t>
+  </si>
+  <si>
+    <t>Segmentation explanation</t>
+  </si>
+  <si>
+    <t>package instructions</t>
+  </si>
+  <si>
+    <t>Final background design</t>
+  </si>
+  <si>
+    <t>Dijkstra scoring</t>
+  </si>
+  <si>
+    <t>Segmentation scoring</t>
+  </si>
+  <si>
+    <t>Sprint 4</t>
   </si>
 </sst>
 </file>
@@ -424,10 +499,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1506,10 +1587,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet2!$G$79:$I$79</c:f>
+              <c:f>Sheet2!$G$79:$J$79</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -1519,15 +1600,18 @@
                 <c:pt idx="2">
                   <c:v>2</c:v>
                 </c:pt>
+                <c:pt idx="3">
+                  <c:v>3</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet2!$G$91:$I$91</c:f>
+              <c:f>Sheet2!$G$91:$J$91</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>63</c:v>
                 </c:pt>
@@ -1536,6 +1620,9 @@
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>41</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>39</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5035,17 +5122,17 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A6:J91"/>
+  <dimension ref="A6:J127"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E65" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="M96" sqref="M96"/>
+    <sheetView tabSelected="1" topLeftCell="B98" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="G112" sqref="G112"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="22.83203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.6640625" customWidth="1"/>
-    <col min="6" max="6" width="27.83203125" customWidth="1"/>
+    <col min="6" max="6" width="29.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="6" spans="1:1" x14ac:dyDescent="0.2">
@@ -5485,8 +5572,11 @@
       <c r="I80">
         <v>0</v>
       </c>
-    </row>
-    <row r="81" spans="6:9" x14ac:dyDescent="0.2">
+      <c r="J80">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="81" spans="6:10" x14ac:dyDescent="0.2">
       <c r="F81" t="s">
         <v>109</v>
       </c>
@@ -5499,8 +5589,11 @@
       <c r="I81">
         <v>4</v>
       </c>
-    </row>
-    <row r="82" spans="6:9" x14ac:dyDescent="0.2">
+      <c r="J81">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="82" spans="6:10" x14ac:dyDescent="0.2">
       <c r="F82" t="s">
         <v>112</v>
       </c>
@@ -5513,8 +5606,11 @@
       <c r="I82">
         <v>8</v>
       </c>
-    </row>
-    <row r="83" spans="6:9" x14ac:dyDescent="0.2">
+      <c r="J82">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="83" spans="6:10" x14ac:dyDescent="0.2">
       <c r="F83" t="s">
         <v>113</v>
       </c>
@@ -5527,8 +5623,11 @@
       <c r="I83">
         <v>0</v>
       </c>
-    </row>
-    <row r="84" spans="6:9" x14ac:dyDescent="0.2">
+      <c r="J83">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="6:10" x14ac:dyDescent="0.2">
       <c r="F84" t="s">
         <v>111</v>
       </c>
@@ -5541,8 +5640,11 @@
       <c r="I84">
         <v>5</v>
       </c>
-    </row>
-    <row r="85" spans="6:9" x14ac:dyDescent="0.2">
+      <c r="J84">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="85" spans="6:10" x14ac:dyDescent="0.2">
       <c r="F85" t="s">
         <v>114</v>
       </c>
@@ -5555,8 +5657,11 @@
       <c r="I85">
         <v>1</v>
       </c>
-    </row>
-    <row r="86" spans="6:9" x14ac:dyDescent="0.2">
+      <c r="J85">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="86" spans="6:10" x14ac:dyDescent="0.2">
       <c r="F86" t="s">
         <v>115</v>
       </c>
@@ -5569,8 +5674,11 @@
       <c r="I86">
         <v>1</v>
       </c>
-    </row>
-    <row r="87" spans="6:9" x14ac:dyDescent="0.2">
+      <c r="J86">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="87" spans="6:10" x14ac:dyDescent="0.2">
       <c r="F87" t="s">
         <v>116</v>
       </c>
@@ -5583,8 +5691,11 @@
       <c r="I87">
         <v>15</v>
       </c>
-    </row>
-    <row r="88" spans="6:9" x14ac:dyDescent="0.2">
+      <c r="J87">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="88" spans="6:10" x14ac:dyDescent="0.2">
       <c r="F88" t="s">
         <v>117</v>
       </c>
@@ -5597,8 +5708,11 @@
       <c r="I88">
         <v>4</v>
       </c>
-    </row>
-    <row r="89" spans="6:9" x14ac:dyDescent="0.2">
+      <c r="J88">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="89" spans="6:10" x14ac:dyDescent="0.2">
       <c r="F89" t="s">
         <v>118</v>
       </c>
@@ -5611,8 +5725,11 @@
       <c r="I89">
         <v>1</v>
       </c>
-    </row>
-    <row r="90" spans="6:9" ht="32" x14ac:dyDescent="0.2">
+      <c r="J89">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="90" spans="6:10" ht="32" x14ac:dyDescent="0.2">
       <c r="F90" s="1" t="s">
         <v>119</v>
       </c>
@@ -5625,8 +5742,11 @@
       <c r="I90">
         <v>2</v>
       </c>
-    </row>
-    <row r="91" spans="6:9" x14ac:dyDescent="0.2">
+      <c r="J90">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="91" spans="6:10" x14ac:dyDescent="0.2">
       <c r="G91">
         <f>SUM(G80:G90)</f>
         <v>63</v>
@@ -5638,6 +5758,255 @@
       <c r="I91">
         <f>SUM(I80:I90)</f>
         <v>41</v>
+      </c>
+      <c r="J91">
+        <f>SUM(J80:J90)</f>
+        <v>39</v>
+      </c>
+    </row>
+    <row r="93" spans="6:10" x14ac:dyDescent="0.2">
+      <c r="F93" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="94" spans="6:10" x14ac:dyDescent="0.2">
+      <c r="F94" t="s">
+        <v>101</v>
+      </c>
+      <c r="G94">
+        <v>0</v>
+      </c>
+      <c r="H94">
+        <v>1</v>
+      </c>
+      <c r="I94">
+        <v>2</v>
+      </c>
+      <c r="J94">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="95" spans="6:10" x14ac:dyDescent="0.2">
+      <c r="F95" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="96" spans="6:10" x14ac:dyDescent="0.2">
+      <c r="F96" t="s">
+        <v>130</v>
+      </c>
+      <c r="G96">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="97" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F97" t="s">
+        <v>115</v>
+      </c>
+      <c r="G97">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="98" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F98" t="s">
+        <v>114</v>
+      </c>
+      <c r="G98">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="99" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F99" t="s">
+        <v>131</v>
+      </c>
+      <c r="G99">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="100" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F100" t="s">
+        <v>133</v>
+      </c>
+      <c r="G100">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="101" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F101" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="102" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F102" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="G102">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="103" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F103" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="G103">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="104" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F104" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="G104">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="105" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F105" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="G105">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="106" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F106" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="G106">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="107" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F107" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="G107">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="108" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F108" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="G108">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="109" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F109" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="G109">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="110" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F110" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="G110">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="111" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F111" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="G111">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="113" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F113" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="114" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F114" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="115" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F115" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="G115">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="116" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F116" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="G116">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="117" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F117" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="G117">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="118" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F118" s="3" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="119" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F119" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="G119">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="120" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F120" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="G120">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="121" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F121" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="G121">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="122" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F122" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="G122">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="123" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F123" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="G123">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="124" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F124" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="G124">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="127" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="G127">
+        <f>SUM(G96:G124)</f>
+        <v>42.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
tried to fix the backgrounds and also wrote the final report
</commit_message>
<xml_diff>
--- a/basic backlog.xlsx
+++ b/basic backlog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/karlypeckham/Dropbox/Grade 16/Semester 2/Senior Project/Senior-Project-Networking-Game/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{DA566CB2-EE17-A04A-B376-0AA98956BF23}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{91B43A03-298E-A242-9CA3-96E717116853}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5860" yWindow="460" windowWidth="22940" windowHeight="17460" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1814,6 +1814,35 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Sprint</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> 4 Burndown</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1852,9 +1881,6 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
-          <c:tx>
-            <c:v>Sprint 4 Burndown</c:v>
-          </c:tx>
           <c:spPr>
             <a:ln w="28575" cap="rnd">
               <a:solidFill>
@@ -1869,30 +1895,42 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet2!$G$94:$H$94</c:f>
+              <c:f>Sheet2!$G$94:$J$94</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="2"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>1</c:v>
                 </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet2!$G$127:$H$127</c:f>
+              <c:f>Sheet2!$G$127:$J$127</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="2"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>42.5</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>36.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>29.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>12</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5008,15 +5046,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>37041</xdr:colOff>
-      <xdr:row>98</xdr:row>
-      <xdr:rowOff>162984</xdr:rowOff>
+      <xdr:colOff>619124</xdr:colOff>
+      <xdr:row>96</xdr:row>
+      <xdr:rowOff>120651</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>481541</xdr:colOff>
-      <xdr:row>112</xdr:row>
-      <xdr:rowOff>91017</xdr:rowOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>238124</xdr:colOff>
+      <xdr:row>110</xdr:row>
+      <xdr:rowOff>48684</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -5309,7 +5347,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D143"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" workbookViewId="0">
+    <sheetView topLeftCell="K18" workbookViewId="0">
       <selection activeCell="A34" sqref="A34:XFD34"/>
     </sheetView>
   </sheetViews>
@@ -5986,8 +6024,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A6:J127"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E92" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="M117" sqref="M117"/>
+    <sheetView tabSelected="1" topLeftCell="E93" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="L98" sqref="L98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6658,8 +6696,14 @@
       <c r="H96">
         <v>2</v>
       </c>
-    </row>
-    <row r="97" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="I96">
+        <v>2</v>
+      </c>
+      <c r="J96">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="6:10" x14ac:dyDescent="0.2">
       <c r="F97" t="s">
         <v>115</v>
       </c>
@@ -6669,8 +6713,14 @@
       <c r="H97">
         <v>1</v>
       </c>
-    </row>
-    <row r="98" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="I97">
+        <v>0</v>
+      </c>
+      <c r="J97">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="6:10" x14ac:dyDescent="0.2">
       <c r="F98" t="s">
         <v>114</v>
       </c>
@@ -6680,8 +6730,14 @@
       <c r="H98">
         <v>1</v>
       </c>
-    </row>
-    <row r="99" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="I98">
+        <v>1</v>
+      </c>
+      <c r="J98">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="6:10" x14ac:dyDescent="0.2">
       <c r="F99" t="s">
         <v>129</v>
       </c>
@@ -6691,8 +6747,14 @@
       <c r="H99">
         <v>4</v>
       </c>
-    </row>
-    <row r="100" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="I99">
+        <v>4</v>
+      </c>
+      <c r="J99">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="6:10" x14ac:dyDescent="0.2">
       <c r="F100" t="s">
         <v>131</v>
       </c>
@@ -6702,13 +6764,19 @@
       <c r="H100">
         <v>4</v>
       </c>
-    </row>
-    <row r="101" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="I100">
+        <v>4</v>
+      </c>
+      <c r="J100">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="6:10" x14ac:dyDescent="0.2">
       <c r="F101" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="102" spans="6:8" x14ac:dyDescent="0.2">
+    <row r="102" spans="6:10" x14ac:dyDescent="0.2">
       <c r="F102" s="2" t="s">
         <v>132</v>
       </c>
@@ -6718,8 +6786,14 @@
       <c r="H102">
         <v>1</v>
       </c>
-    </row>
-    <row r="103" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="I102">
+        <v>0</v>
+      </c>
+      <c r="J102">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103" spans="6:10" x14ac:dyDescent="0.2">
       <c r="F103" s="2" t="s">
         <v>133</v>
       </c>
@@ -6729,8 +6803,14 @@
       <c r="H103">
         <v>1</v>
       </c>
-    </row>
-    <row r="104" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="I103">
+        <v>0</v>
+      </c>
+      <c r="J103">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104" spans="6:10" x14ac:dyDescent="0.2">
       <c r="F104" s="2" t="s">
         <v>134</v>
       </c>
@@ -6740,8 +6820,14 @@
       <c r="H104">
         <v>1</v>
       </c>
-    </row>
-    <row r="105" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="I104">
+        <v>0</v>
+      </c>
+      <c r="J104">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" spans="6:10" x14ac:dyDescent="0.2">
       <c r="F105" s="2" t="s">
         <v>135</v>
       </c>
@@ -6751,8 +6837,14 @@
       <c r="H105">
         <v>0</v>
       </c>
-    </row>
-    <row r="106" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="I105">
+        <v>0</v>
+      </c>
+      <c r="J105">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106" spans="6:10" x14ac:dyDescent="0.2">
       <c r="F106" s="2" t="s">
         <v>136</v>
       </c>
@@ -6762,8 +6854,14 @@
       <c r="H106">
         <v>0</v>
       </c>
-    </row>
-    <row r="107" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="I106">
+        <v>0</v>
+      </c>
+      <c r="J106">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="107" spans="6:10" x14ac:dyDescent="0.2">
       <c r="F107" s="2" t="s">
         <v>137</v>
       </c>
@@ -6773,8 +6871,14 @@
       <c r="H107">
         <v>0</v>
       </c>
-    </row>
-    <row r="108" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="I107">
+        <v>0</v>
+      </c>
+      <c r="J107">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="108" spans="6:10" x14ac:dyDescent="0.2">
       <c r="F108" s="2" t="s">
         <v>138</v>
       </c>
@@ -6784,8 +6888,14 @@
       <c r="H108">
         <v>0</v>
       </c>
-    </row>
-    <row r="109" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="I108">
+        <v>0</v>
+      </c>
+      <c r="J108">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="109" spans="6:10" x14ac:dyDescent="0.2">
       <c r="F109" s="3" t="s">
         <v>139</v>
       </c>
@@ -6795,8 +6905,14 @@
       <c r="H109">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="110" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="I109">
+        <v>0</v>
+      </c>
+      <c r="J109">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="110" spans="6:10" x14ac:dyDescent="0.2">
       <c r="F110" s="3" t="s">
         <v>140</v>
       </c>
@@ -6806,8 +6922,14 @@
       <c r="H110">
         <v>3</v>
       </c>
-    </row>
-    <row r="111" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="I110">
+        <v>3</v>
+      </c>
+      <c r="J110">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="111" spans="6:10" x14ac:dyDescent="0.2">
       <c r="F111" s="3" t="s">
         <v>141</v>
       </c>
@@ -6817,13 +6939,19 @@
       <c r="H111">
         <v>3</v>
       </c>
-    </row>
-    <row r="114" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="I111">
+        <v>4</v>
+      </c>
+      <c r="J111">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="114" spans="6:10" x14ac:dyDescent="0.2">
       <c r="F114" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="115" spans="6:8" x14ac:dyDescent="0.2">
+    <row r="115" spans="6:10" x14ac:dyDescent="0.2">
       <c r="F115" s="2" t="s">
         <v>120</v>
       </c>
@@ -6833,8 +6961,14 @@
       <c r="H115">
         <v>0</v>
       </c>
-    </row>
-    <row r="116" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="I115">
+        <v>0</v>
+      </c>
+      <c r="J115">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="116" spans="6:10" x14ac:dyDescent="0.2">
       <c r="F116" s="2" t="s">
         <v>121</v>
       </c>
@@ -6844,8 +6978,14 @@
       <c r="H116">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="117" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="I116">
+        <v>0.5</v>
+      </c>
+      <c r="J116">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="117" spans="6:10" x14ac:dyDescent="0.2">
       <c r="F117" s="2" t="s">
         <v>122</v>
       </c>
@@ -6855,13 +6995,19 @@
       <c r="H117">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="118" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="I117">
+        <v>1</v>
+      </c>
+      <c r="J117">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="118" spans="6:10" x14ac:dyDescent="0.2">
       <c r="F118" s="3" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="119" spans="6:8" x14ac:dyDescent="0.2">
+    <row r="119" spans="6:10" x14ac:dyDescent="0.2">
       <c r="F119" s="2" t="s">
         <v>123</v>
       </c>
@@ -6871,8 +7017,14 @@
       <c r="H119">
         <v>2</v>
       </c>
-    </row>
-    <row r="120" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="I119">
+        <v>4</v>
+      </c>
+      <c r="J119">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="120" spans="6:10" x14ac:dyDescent="0.2">
       <c r="F120" s="2" t="s">
         <v>124</v>
       </c>
@@ -6882,8 +7034,14 @@
       <c r="H120">
         <v>4</v>
       </c>
-    </row>
-    <row r="121" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="I120">
+        <v>4</v>
+      </c>
+      <c r="J120">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="121" spans="6:10" x14ac:dyDescent="0.2">
       <c r="F121" s="2" t="s">
         <v>125</v>
       </c>
@@ -6893,8 +7051,14 @@
       <c r="H121">
         <v>2</v>
       </c>
-    </row>
-    <row r="122" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="I121">
+        <v>1</v>
+      </c>
+      <c r="J121">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="122" spans="6:10" x14ac:dyDescent="0.2">
       <c r="F122" s="2" t="s">
         <v>126</v>
       </c>
@@ -6904,8 +7068,14 @@
       <c r="H122">
         <v>1</v>
       </c>
-    </row>
-    <row r="123" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="I122">
+        <v>1</v>
+      </c>
+      <c r="J122">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="123" spans="6:10" x14ac:dyDescent="0.2">
       <c r="F123" s="3" t="s">
         <v>127</v>
       </c>
@@ -6915,8 +7085,14 @@
       <c r="H123">
         <v>1</v>
       </c>
-    </row>
-    <row r="124" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="I123">
+        <v>0</v>
+      </c>
+      <c r="J123">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="124" spans="6:10" x14ac:dyDescent="0.2">
       <c r="F124" s="3" t="s">
         <v>130</v>
       </c>
@@ -6926,8 +7102,14 @@
       <c r="H124">
         <v>4</v>
       </c>
-    </row>
-    <row r="127" spans="6:8" x14ac:dyDescent="0.2">
+      <c r="I124">
+        <v>0</v>
+      </c>
+      <c r="J124">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="127" spans="6:10" x14ac:dyDescent="0.2">
       <c r="G127">
         <f>SUM(G96:G124)</f>
         <v>42.5</v>
@@ -6935,6 +7117,14 @@
       <c r="H127">
         <f>SUM(H96:H124)</f>
         <v>36.5</v>
+      </c>
+      <c r="I127">
+        <f>SUM(I96:I124)</f>
+        <v>29.5</v>
+      </c>
+      <c r="J127">
+        <f>SUM(J96:J124)</f>
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>